<commit_message>
loopas skyriam, pagination, turinys, titulinis edited, nuotrauku pridejimas
</commit_message>
<xml_diff>
--- a/Duomenys.xlsx
+++ b/Duomenys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aido\2 Kursas\2 pusmetis\VPR\Darbai\BakalauroStruktura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e796dfc644230e08/Documents/UiPath/vpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532FCCB9-86D8-4130-8550-65598D61FF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{532FCCB9-86D8-4130-8550-65598D61FF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4900850-2215-4FB5-9F39-58368E670AE7}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="120" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagrindinis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Universitetas</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Duomenu bazių struktūros tyrimas</t>
+  </si>
+  <si>
+    <t>Miestas</t>
+  </si>
+  <si>
+    <t>Vilnius</t>
   </si>
 </sst>
 </file>
@@ -120,12 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -403,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +425,7 @@
     <col min="6" max="8" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +450,11 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -468,6 +478,9 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>